<commit_message>
payment mode added on export
</commit_message>
<xml_diff>
--- a/exports/off-bridges_report.xlsx
+++ b/exports/off-bridges_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>NumRef</t>
   </si>
@@ -62,6 +62,45 @@
   </si>
   <si>
     <t>Initier par</t>
+  </si>
+  <si>
+    <t>03250002</t>
+  </si>
+  <si>
+    <t>Cause incident 1</t>
+  </si>
+  <si>
+    <t>SALLE DE CONFERENCE ROOM</t>
+  </si>
+  <si>
+    <t>2NT</t>
+  </si>
+  <si>
+    <t>plomb 1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>:ETS DJOUBISSIE ET FILS</t>
+  </si>
+  <si>
+    <t>(CETOSTEARYL ALCOHOL</t>
+  </si>
+  <si>
+    <t>13 BSMAT GAP MCD MOULINS</t>
+  </si>
+  <si>
+    <t>O45FFG</t>
+  </si>
+  <si>
+    <t>ALI</t>
+  </si>
+  <si>
+    <t>455RG</t>
+  </si>
+  <si>
+    <t>Admin User</t>
   </si>
 </sst>
 </file>
@@ -438,7 +477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:Q2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -498,6 +537,47 @@
         <v>16</v>
       </c>
     </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>